<commit_message>
dados complementares adicionados no codigo, exceto dados do docente
</commit_message>
<xml_diff>
--- a/new_data_dd.xlsx
+++ b/new_data_dd.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marcos\Documents\planilha_controle_dd_iesb\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\www\IESB\planilha_controle_dd_iesb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAFF7275-9EFE-4188-B4BA-AAC8DB723F8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{032972BC-64B9-4F83-8ACC-2A86984DDABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$F$18</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,9 +26,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -38,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="46">
   <si>
     <t>CAMPO</t>
   </si>
@@ -173,6 +171,9 @@
   </si>
   <si>
     <t>VW_CONSULTA_DIPLOMA_ATV_COMPLEMENTAR</t>
+  </si>
+  <si>
+    <t>Dados da View adicionados no código</t>
   </si>
 </sst>
 </file>
@@ -604,7 +605,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -955,9 +956,11 @@
         <v>44</v>
       </c>
       <c r="D20" s="2"/>
-      <c r="E20" s="3"/>
+      <c r="E20" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="F20" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
ajuste codigo - dados de estagio e atv
</commit_message>
<xml_diff>
--- a/new_data_dd.xlsx
+++ b/new_data_dd.xlsx
@@ -5,18 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marcos\Documents\planilha_controle_dd_iesb\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\www\IESB\planilha_controle_dd_iesb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82FB6E70-8869-4B84-92B7-A1DAF9813320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7787B02-6D4A-4F16-801E-B53F82DEAFD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$F$18</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$G$18</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="48">
   <si>
     <t>CAMPO</t>
   </si>
@@ -107,9 +107,6 @@
     <t>Período letivo do aluno: Campo texto para informar o período letivo do aluno</t>
   </si>
   <si>
-    <t>AJUSTADO</t>
-  </si>
-  <si>
     <t>Estrutura nova para o campo aluSituacaoENADE (Enade)</t>
   </si>
   <si>
@@ -177,6 +174,12 @@
   </si>
   <si>
     <t>VW_CONSULTA_DIPLOMA_ESTAGIO</t>
+  </si>
+  <si>
+    <t>AJUSTADO NO BD</t>
+  </si>
+  <si>
+    <t>AJUSTADO NO CODIGO</t>
   </si>
 </sst>
 </file>
@@ -605,22 +608,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="76.42578125" style="5" customWidth="1"/>
     <col min="4" max="4" width="76.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="79.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -631,16 +636,19 @@
         <v>3</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -651,14 +659,17 @@
         <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E2" s="3"/>
-      <c r="F2" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -669,14 +680,17 @@
         <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E3" s="3"/>
-      <c r="F3" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -687,14 +701,17 @@
         <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E4" s="3"/>
-      <c r="F4" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
@@ -705,14 +722,17 @@
         <v>12</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E5" s="3"/>
-      <c r="F5" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
@@ -723,14 +743,17 @@
         <v>15</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E6" s="3"/>
-      <c r="F6" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
@@ -741,16 +764,19 @@
         <v>17</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>19</v>
       </c>
@@ -759,16 +785,19 @@
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>20</v>
       </c>
@@ -777,16 +806,19 @@
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>21</v>
       </c>
@@ -797,194 +829,224 @@
         <v>22</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E10" s="3"/>
-      <c r="F10" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E16" s="3"/>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F16" s="3"/>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E17" s="3"/>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F17" s="3"/>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="2"/>
       <c r="C19" s="3"/>
       <c r="D19" s="2"/>
       <c r="E19" s="3"/>
-      <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F19" s="3"/>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="3"/>
       <c r="F21" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>7</v>
@@ -995,10 +1057,13 @@
       <c r="F22" s="6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>7</v>
@@ -1009,95 +1074,108 @@
       <c r="F23" s="6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="2"/>
       <c r="C24" s="3"/>
       <c r="D24" s="2"/>
       <c r="E24" s="3"/>
-      <c r="F24" s="2"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F24" s="3"/>
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="2"/>
       <c r="C25" s="3"/>
       <c r="D25" s="2"/>
       <c r="E25" s="3"/>
-      <c r="F25" s="2"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F25" s="3"/>
+      <c r="G25" s="2"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
       <c r="D26" s="2"/>
       <c r="E26" s="3"/>
-      <c r="F26" s="2"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F26" s="3"/>
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
       <c r="D27" s="2"/>
       <c r="E27" s="3"/>
-      <c r="F27" s="2"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F27" s="3"/>
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
       <c r="D28" s="2"/>
       <c r="E28" s="3"/>
-      <c r="F28" s="2"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F28" s="3"/>
+      <c r="G28" s="2"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
       <c r="D29" s="2"/>
       <c r="E29" s="3"/>
-      <c r="F29" s="2"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F29" s="3"/>
+      <c r="G29" s="2"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="2"/>
       <c r="C30" s="3"/>
       <c r="D30" s="2"/>
       <c r="E30" s="3"/>
-      <c r="F30" s="2"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F30" s="3"/>
+      <c r="G30" s="2"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="2"/>
       <c r="C31" s="3"/>
       <c r="D31" s="2"/>
       <c r="E31" s="3"/>
-      <c r="F31" s="2"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F31" s="3"/>
+      <c r="G31" s="2"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="2"/>
       <c r="C32" s="3"/>
       <c r="D32" s="2"/>
       <c r="E32" s="3"/>
-      <c r="F32" s="2"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F32" s="3"/>
+      <c r="G32" s="2"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="2"/>
       <c r="C33" s="3"/>
       <c r="D33" s="2"/>
       <c r="E33" s="3"/>
-      <c r="F33" s="2"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F18" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:G18" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <mergeCells count="1">
     <mergeCell ref="A26:C29"/>
   </mergeCells>
-  <conditionalFormatting sqref="F2:F15 A30:E33 A26 D26:E29 A2:E25">
+  <conditionalFormatting sqref="G2:G15 A30:F33 A26 D26:F29 A2:F19 A22:F25 A20:E21">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"NÃO"</formula>
     </cfRule>
@@ -1105,7 +1183,7 @@
       <formula>"SIM"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F18">
+  <conditionalFormatting sqref="G18">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"NÃO"</formula>
     </cfRule>
@@ -1113,7 +1191,7 @@
       <formula>"SIM"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F20:F23">
+  <conditionalFormatting sqref="G22:G23 F20:G21">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"NÃO"</formula>
     </cfRule>

</xml_diff>

<commit_message>
ultimos ajustes em codigo
</commit_message>
<xml_diff>
--- a/new_data_dd.xlsx
+++ b/new_data_dd.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marcos\Documents\planilha_controle_dd_iesb\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\www\IESB\planilha_controle_dd_iesb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B1D7B9-077B-458F-809A-F2ED4660130E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F29F92E0-158B-4360-9352-F0AC9376F741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="15600" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="51">
   <si>
     <t>CAMPO</t>
   </si>
@@ -189,13 +189,39 @@
   </si>
   <si>
     <t>VW_CONSULTA_DIPLOMA_ASSINANTES_DIPLOMA</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">o Campo </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>hisSituacao</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> não foi ajustado na base</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,6 +233,21 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -226,7 +267,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -249,11 +290,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -280,13 +401,80 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -626,7 +814,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="A30" sqref="A30:C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -678,10 +866,10 @@
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -699,10 +887,10 @@
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -720,10 +908,10 @@
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -741,10 +929,10 @@
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -762,10 +950,10 @@
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -785,10 +973,10 @@
         <v>18</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -806,10 +994,10 @@
         <v>18</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -827,10 +1015,10 @@
         <v>18</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1000,7 +1188,9 @@
         <v>33</v>
       </c>
       <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
+      <c r="F17" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="G17" s="6" t="s">
         <v>6</v>
       </c>
@@ -1088,7 +1278,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="3"/>
       <c r="F22" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G22" s="6" t="s">
         <v>6</v>
@@ -1107,7 +1297,7 @@
       <c r="D23" s="2"/>
       <c r="E23" s="3"/>
       <c r="F23" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G23" s="6" t="s">
         <v>6</v>
@@ -1170,27 +1360,29 @@
       <c r="G29" s="2"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="3"/>
+      <c r="A30" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" s="11"/>
+      <c r="C30" s="12"/>
       <c r="D30" s="2"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
       <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="3"/>
+      <c r="A31" s="13"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="15"/>
       <c r="D31" s="2"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
       <c r="G31" s="2"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="3"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="3"/>
+      <c r="A32" s="16"/>
+      <c r="B32" s="17"/>
+      <c r="C32" s="18"/>
       <c r="D32" s="2"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
@@ -1207,33 +1399,51 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:G18" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A26:C29"/>
+    <mergeCell ref="A30:C32"/>
   </mergeCells>
-  <conditionalFormatting sqref="A30:F33 A26 D26:F29 A22:F25 A20:E21 A2:F19 G2:G17">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+  <conditionalFormatting sqref="A33:F33 A26 A24:F25 A20:E23 A7:F19 G7:G17 A2:E6 A30 D26:F32">
+    <cfRule type="cellIs" dxfId="1" priority="9" operator="equal">
       <formula>"NÃO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="10" operator="equal">
       <formula>"SIM"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G18">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
       <formula>"NÃO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
       <formula>"SIM"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G22:G23 F20:G21">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+  <conditionalFormatting sqref="F20:G23">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
       <formula>"NÃO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+      <formula>"SIM"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:G2">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+      <formula>"NÃO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+      <formula>"SIM"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3:G6">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"NÃO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"SIM"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
campos que não existem no codigo
</commit_message>
<xml_diff>
--- a/new_data_dd.xlsx
+++ b/new_data_dd.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\www\IESB\planilha_controle_dd_iesb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F29F92E0-158B-4360-9352-F0AC9376F741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B36FE08-A1DE-4B42-937E-00332BDCED8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="15600" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="15600" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$G$18</definedName>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="57">
   <si>
     <t>CAMPO</t>
   </si>
@@ -215,6 +216,44 @@
       </rPr>
       <t xml:space="preserve"> não foi ajustado na base</t>
     </r>
+  </si>
+  <si>
+    <t>idTemplate</t>
+  </si>
+  <si>
+    <t>Habilitacoes</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 1 - curRecDataProtocolo </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>existe no exemplo de json, mas não há detalhamento do campo na documentação.</t>
+    </r>
+  </si>
+  <si>
+    <t>NÃO EXISTE NO CODIGO</t>
+  </si>
+  <si>
+    <t>Enfase</t>
+  </si>
+  <si>
+    <t>Campo add no codigo, porém é passado vazio</t>
   </si>
 </sst>
 </file>
@@ -374,7 +413,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -430,6 +469,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -813,8 +856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:C32"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1404,46 +1447,140 @@
     <mergeCell ref="A30:C32"/>
   </mergeCells>
   <conditionalFormatting sqref="A33:F33 A26 A24:F25 A20:E23 A7:F19 G7:G17 A2:E6 A30 D26:F32">
-    <cfRule type="cellIs" dxfId="1" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>"NÃO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
       <formula>"SIM"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G18">
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>"NÃO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
       <formula>"SIM"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20:G23">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"NÃO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>"SIM"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:G2">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"NÃO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"SIM"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:G6">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"NÃO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"SIM"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B9088FA-E1FB-463F-A59C-064F0CAFCF7D}">
+  <dimension ref="A1:M15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H11" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="19"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="19"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="19"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="19"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="19"/>
+      <c r="M15" s="19"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H11:M15"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>